<commit_message>
update to sample_products to avoid upload issues
</commit_message>
<xml_diff>
--- a/cypress/assets/sample_product.xlsx
+++ b/cypress/assets/sample_product.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anneikaweeks/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anneikaweeks/Documents/cypress/cypress/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F59C04A1-38C5-3F42-BCE7-32C854CA935E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58CB3F7A-FE8B-4849-BDE4-10E60A06D8CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="780" windowWidth="16380" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -444,7 +444,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -477,7 +477,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>2</v>

</xml_diff>